<commit_message>
Fixing bug with correctly accounting for unlimited datasets
</commit_message>
<xml_diff>
--- a/tests/validation_results/Validation_Inputs_Loci100mutual.xlsx
+++ b/tests/validation_results/Validation_Inputs_Loci100mutual.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B4D9B2-9EF8-4F62-9C6B-C224333C4E44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F60F1B-D19B-4E8C-A454-1C58CD94B591}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36240" yWindow="2775" windowWidth="21600" windowHeight="11385" tabRatio="814" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="814" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -1178,9 +1178,6 @@
     <t>Study Settings</t>
   </si>
   <si>
-    <t>Results_</t>
-  </si>
-  <si>
     <t xml:space="preserve">	ldf.iopt_net </t>
   </si>
   <si>
@@ -2589,6 +2586,9 @@
   </si>
   <si>
     <t>4973328_KTS_DPTS_2 220kV</t>
+  </si>
+  <si>
+    <t>Res_C100_Z12_AllPoint_V15</t>
   </si>
 </sst>
 </file>
@@ -4517,7 +4517,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B1" s="78"/>
       <c r="C1" s="78"/>
@@ -4525,17 +4525,17 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="78" t="s">
         <v>196</v>
-      </c>
-      <c r="B2" s="78" t="s">
-        <v>197</v>
       </c>
       <c r="C2" s="78"/>
       <c r="D2" s="78"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="79" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B3" s="79"/>
       <c r="C3" s="79"/>
@@ -4543,7 +4543,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="80" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B4" s="80"/>
       <c r="C4" s="80"/>
@@ -4571,44 +4571,44 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" s="8">
         <v>43977</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C8" s="8">
         <v>44015</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C9" s="8">
         <v>44030</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4785,7 +4785,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -4806,7 +4806,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="84" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B2" s="84"/>
       <c r="C2" s="84"/>
@@ -4826,101 +4826,101 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>25</v>
+        <v>495</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B7" s="34" t="b">
         <v>1</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B8" s="34" t="b">
         <v>0</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B9" s="34" t="b">
         <v>1</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B10" s="34" t="b">
         <v>1</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B11" s="34" t="b">
         <v>1</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B12" s="34" t="b">
         <v>1</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B13" s="34" t="b">
         <v>1</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -5005,44 +5005,44 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>239</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="C5" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" s="22" t="s">
         <v>240</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="C6" s="22" t="s">
         <v>242</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="C6" s="22" t="s">
+      <c r="D6" s="22" t="s">
         <v>243</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="C7" s="22" t="s">
         <v>245</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="C7" s="22" t="s">
+      <c r="D7" s="22" t="s">
         <v>246</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5174,7 +5174,7 @@
   <sheetData>
     <row r="1" spans="1:28" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="87" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B1" s="87"/>
       <c r="C1" s="83"/>
@@ -5236,13 +5236,13 @@
     </row>
     <row r="3" spans="1:28" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="53" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="54" t="s">
         <v>188</v>
-      </c>
-      <c r="B3" s="54" t="s">
-        <v>190</v>
-      </c>
-      <c r="C3" s="54" t="s">
-        <v>189</v>
       </c>
       <c r="D3" s="53" t="b">
         <v>0</v>
@@ -5250,7 +5250,7 @@
     </row>
     <row r="4" spans="1:28" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B4" s="92" t="s">
         <v>6</v>
@@ -5309,7 +5309,7 @@
         <v>16</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E5" s="29" t="s">
         <v>15</v>
@@ -5318,7 +5318,7 @@
         <v>16</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H5" s="29" t="s">
         <v>15</v>
@@ -5327,7 +5327,7 @@
         <v>16</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K5" s="29" t="s">
         <v>15</v>
@@ -5336,7 +5336,7 @@
         <v>16</v>
       </c>
       <c r="M5" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N5" s="29" t="s">
         <v>15</v>
@@ -5345,7 +5345,7 @@
         <v>16</v>
       </c>
       <c r="P5" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q5" s="29" t="s">
         <v>15</v>
@@ -5354,7 +5354,7 @@
         <v>16</v>
       </c>
       <c r="S5" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="T5" s="29" t="s">
         <v>15</v>
@@ -5363,7 +5363,7 @@
         <v>16</v>
       </c>
       <c r="V5" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="W5" s="29" t="s">
         <v>15</v>
@@ -5372,7 +5372,7 @@
         <v>16</v>
       </c>
       <c r="Y5" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Z5" s="29" t="s">
         <v>15</v>
@@ -5381,21 +5381,21 @@
         <v>16</v>
       </c>
       <c r="AB5" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="C6" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>250</v>
-      </c>
       <c r="D6" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
@@ -5424,25 +5424,25 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="C7" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="D7" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="F7" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>252</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>254</v>
-      </c>
       <c r="G7" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
@@ -10321,7 +10321,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="84" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="95" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="83"/>
@@ -10365,13 +10365,13 @@
     </row>
     <row r="3" spans="1:19" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="53" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="52" t="s">
         <v>188</v>
-      </c>
-      <c r="B3" s="51" t="s">
-        <v>190</v>
-      </c>
-      <c r="C3" s="52" t="s">
-        <v>189</v>
       </c>
       <c r="D3" s="50" t="b">
         <v>0</v>
@@ -10379,42 +10379,42 @@
     </row>
     <row r="4" spans="1:19" s="46" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B4" s="92" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C4" s="94"/>
       <c r="D4" s="89" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E4" s="91"/>
       <c r="F4" s="89" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G4" s="91"/>
       <c r="H4" s="89" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I4" s="91"/>
       <c r="J4" s="89" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K4" s="91"/>
       <c r="L4" s="89" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M4" s="91"/>
       <c r="N4" s="89" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O4" s="91"/>
       <c r="P4" s="89" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Q4" s="91"/>
       <c r="R4" s="89" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="S4" s="91"/>
     </row>
@@ -10423,69 +10423,69 @@
         <v>0</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J5" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K5" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L5" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M5" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N5" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O5" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P5" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Q5" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R5" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="S5" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
@@ -10506,13 +10506,13 @@
     </row>
     <row r="7" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
@@ -10533,13 +10533,13 @@
     </row>
     <row r="8" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
@@ -10560,13 +10560,13 @@
     </row>
     <row r="9" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
@@ -10587,13 +10587,13 @@
     </row>
     <row r="10" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
@@ -10614,13 +10614,13 @@
     </row>
     <row r="11" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
@@ -10641,13 +10641,13 @@
     </row>
     <row r="12" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
@@ -10668,13 +10668,13 @@
     </row>
     <row r="13" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
@@ -10695,13 +10695,13 @@
     </row>
     <row r="14" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
@@ -10722,13 +10722,13 @@
     </row>
     <row r="15" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="B15" t="s">
         <v>264</v>
       </c>
-      <c r="B15" t="s">
-        <v>265</v>
-      </c>
       <c r="C15" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
@@ -10749,13 +10749,13 @@
     </row>
     <row r="16" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="B16" t="s">
         <v>279</v>
       </c>
-      <c r="B16" t="s">
-        <v>280</v>
-      </c>
       <c r="C16" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
@@ -10776,13 +10776,13 @@
     </row>
     <row r="17" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="B17" t="s">
         <v>281</v>
       </c>
-      <c r="B17" t="s">
-        <v>282</v>
-      </c>
       <c r="C17" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
@@ -10803,13 +10803,13 @@
     </row>
     <row r="18" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="B18" t="s">
         <v>283</v>
       </c>
-      <c r="B18" t="s">
-        <v>284</v>
-      </c>
       <c r="C18" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
@@ -10830,13 +10830,13 @@
     </row>
     <row r="19" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="B19" t="s">
         <v>285</v>
       </c>
-      <c r="B19" t="s">
-        <v>286</v>
-      </c>
       <c r="C19" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="18"/>
@@ -10857,13 +10857,13 @@
     </row>
     <row r="20" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="B20" t="s">
         <v>287</v>
       </c>
-      <c r="B20" t="s">
-        <v>288</v>
-      </c>
       <c r="C20" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D20" s="18"/>
       <c r="E20" s="18"/>
@@ -10884,13 +10884,13 @@
     </row>
     <row r="21" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="B21" t="s">
         <v>289</v>
       </c>
-      <c r="B21" t="s">
-        <v>290</v>
-      </c>
       <c r="C21" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D21" s="18"/>
       <c r="E21" s="18"/>
@@ -10911,13 +10911,13 @@
     </row>
     <row r="22" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="B22" t="s">
         <v>291</v>
       </c>
-      <c r="B22" t="s">
-        <v>292</v>
-      </c>
       <c r="C22" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
@@ -10938,13 +10938,13 @@
     </row>
     <row r="23" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
+        <v>292</v>
+      </c>
+      <c r="B23" t="s">
         <v>293</v>
       </c>
-      <c r="B23" t="s">
-        <v>294</v>
-      </c>
       <c r="C23" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
@@ -10965,13 +10965,13 @@
     </row>
     <row r="24" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="B24" t="s">
         <v>295</v>
       </c>
-      <c r="B24" t="s">
-        <v>296</v>
-      </c>
       <c r="C24" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="18"/>
@@ -10992,13 +10992,13 @@
     </row>
     <row r="25" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="B25" t="s">
         <v>297</v>
       </c>
-      <c r="B25" t="s">
-        <v>298</v>
-      </c>
       <c r="C25" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="18"/>
@@ -11019,13 +11019,13 @@
     </row>
     <row r="26" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="B26" t="s">
         <v>299</v>
       </c>
-      <c r="B26" t="s">
-        <v>300</v>
-      </c>
       <c r="C26" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
@@ -11046,13 +11046,13 @@
     </row>
     <row r="27" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="B27" t="s">
         <v>301</v>
       </c>
-      <c r="B27" t="s">
-        <v>302</v>
-      </c>
       <c r="C27" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
@@ -11073,13 +11073,13 @@
     </row>
     <row r="28" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B28" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D28" s="18"/>
       <c r="E28" s="18"/>
@@ -11100,13 +11100,13 @@
     </row>
     <row r="29" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
+        <v>303</v>
+      </c>
+      <c r="B29" t="s">
         <v>304</v>
       </c>
-      <c r="B29" t="s">
-        <v>305</v>
-      </c>
       <c r="C29" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D29" s="18"/>
       <c r="E29" s="18"/>
@@ -11127,13 +11127,13 @@
     </row>
     <row r="30" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="B30" t="s">
         <v>306</v>
       </c>
-      <c r="B30" t="s">
-        <v>307</v>
-      </c>
       <c r="C30" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
@@ -11154,13 +11154,13 @@
     </row>
     <row r="31" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
+        <v>307</v>
+      </c>
+      <c r="B31" t="s">
         <v>308</v>
       </c>
-      <c r="B31" t="s">
-        <v>309</v>
-      </c>
       <c r="C31" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -11181,13 +11181,13 @@
     </row>
     <row r="32" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B32" t="s">
         <v>310</v>
       </c>
-      <c r="B32" t="s">
-        <v>311</v>
-      </c>
       <c r="C32" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
@@ -11208,13 +11208,13 @@
     </row>
     <row r="33" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="B33" t="s">
         <v>312</v>
       </c>
-      <c r="B33" t="s">
-        <v>313</v>
-      </c>
       <c r="C33" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
@@ -11235,13 +11235,13 @@
     </row>
     <row r="34" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="B34" t="s">
         <v>314</v>
       </c>
-      <c r="B34" t="s">
-        <v>315</v>
-      </c>
       <c r="C34" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
@@ -11262,13 +11262,13 @@
     </row>
     <row r="35" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="B35" t="s">
         <v>316</v>
       </c>
-      <c r="B35" t="s">
-        <v>317</v>
-      </c>
       <c r="C35" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D35" s="18"/>
       <c r="E35" s="18"/>
@@ -11289,13 +11289,13 @@
     </row>
     <row r="36" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
+        <v>317</v>
+      </c>
+      <c r="B36" t="s">
         <v>318</v>
       </c>
-      <c r="B36" t="s">
-        <v>319</v>
-      </c>
       <c r="C36" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
@@ -11316,13 +11316,13 @@
     </row>
     <row r="37" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="B37" t="s">
         <v>320</v>
       </c>
-      <c r="B37" t="s">
-        <v>321</v>
-      </c>
       <c r="C37" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D37" s="18"/>
       <c r="E37" s="18"/>
@@ -11343,13 +11343,13 @@
     </row>
     <row r="38" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="B38" t="s">
         <v>322</v>
       </c>
-      <c r="B38" t="s">
-        <v>323</v>
-      </c>
       <c r="C38" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>
@@ -11370,13 +11370,13 @@
     </row>
     <row r="39" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
+        <v>323</v>
+      </c>
+      <c r="B39" t="s">
         <v>324</v>
       </c>
-      <c r="B39" t="s">
-        <v>325</v>
-      </c>
       <c r="C39" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D39" s="18"/>
       <c r="E39" s="18"/>
@@ -11397,13 +11397,13 @@
     </row>
     <row r="40" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="B40" t="s">
         <v>326</v>
       </c>
-      <c r="B40" t="s">
-        <v>327</v>
-      </c>
       <c r="C40" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D40" s="18"/>
       <c r="E40" s="18"/>
@@ -11424,13 +11424,13 @@
     </row>
     <row r="41" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="B41" t="s">
         <v>328</v>
       </c>
-      <c r="B41" t="s">
-        <v>329</v>
-      </c>
       <c r="C41" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D41" s="18"/>
       <c r="E41" s="18"/>
@@ -11451,13 +11451,13 @@
     </row>
     <row r="42" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="B42" t="s">
         <v>330</v>
       </c>
-      <c r="B42" t="s">
-        <v>331</v>
-      </c>
       <c r="C42" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -11478,13 +11478,13 @@
     </row>
     <row r="43" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="B43" t="s">
         <v>332</v>
       </c>
-      <c r="B43" t="s">
-        <v>333</v>
-      </c>
       <c r="C43" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
@@ -11505,13 +11505,13 @@
     </row>
     <row r="44" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
+        <v>333</v>
+      </c>
+      <c r="B44" t="s">
         <v>334</v>
       </c>
-      <c r="B44" t="s">
-        <v>335</v>
-      </c>
       <c r="C44" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D44" s="18"/>
       <c r="E44" s="18"/>
@@ -11532,13 +11532,13 @@
     </row>
     <row r="45" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="B45" t="s">
         <v>336</v>
       </c>
-      <c r="B45" t="s">
-        <v>337</v>
-      </c>
       <c r="C45" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
@@ -11559,13 +11559,13 @@
     </row>
     <row r="46" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="B46" t="s">
         <v>338</v>
       </c>
-      <c r="B46" t="s">
-        <v>339</v>
-      </c>
       <c r="C46" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D46" s="18"/>
       <c r="E46" s="18"/>
@@ -11586,13 +11586,13 @@
     </row>
     <row r="47" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="B47" t="s">
         <v>340</v>
       </c>
-      <c r="B47" t="s">
-        <v>341</v>
-      </c>
       <c r="C47" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D47" s="18"/>
       <c r="E47" s="18"/>
@@ -11613,13 +11613,13 @@
     </row>
     <row r="48" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="B48" t="s">
         <v>342</v>
       </c>
-      <c r="B48" t="s">
-        <v>343</v>
-      </c>
       <c r="C48" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D48" s="18"/>
       <c r="E48" s="18"/>
@@ -11640,13 +11640,13 @@
     </row>
     <row r="49" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
+        <v>343</v>
+      </c>
+      <c r="B49" t="s">
         <v>344</v>
       </c>
-      <c r="B49" t="s">
-        <v>345</v>
-      </c>
       <c r="C49" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D49" s="18"/>
       <c r="E49" s="18"/>
@@ -11667,13 +11667,13 @@
     </row>
     <row r="50" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="B50" t="s">
         <v>346</v>
       </c>
-      <c r="B50" t="s">
-        <v>347</v>
-      </c>
       <c r="C50" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D50" s="18"/>
       <c r="E50" s="18"/>
@@ -11694,13 +11694,13 @@
     </row>
     <row r="51" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="B51" t="s">
         <v>348</v>
       </c>
-      <c r="B51" t="s">
-        <v>349</v>
-      </c>
       <c r="C51" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D51" s="18"/>
       <c r="E51" s="18"/>
@@ -11721,13 +11721,13 @@
     </row>
     <row r="52" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="B52" t="s">
         <v>350</v>
       </c>
-      <c r="B52" t="s">
-        <v>351</v>
-      </c>
       <c r="C52" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D52" s="18"/>
       <c r="E52" s="18"/>
@@ -11748,13 +11748,13 @@
     </row>
     <row r="53" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="B53" t="s">
         <v>352</v>
       </c>
-      <c r="B53" t="s">
-        <v>353</v>
-      </c>
       <c r="C53" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D53" s="18"/>
       <c r="E53" s="18"/>
@@ -11775,13 +11775,13 @@
     </row>
     <row r="54" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="B54" t="s">
         <v>354</v>
       </c>
-      <c r="B54" t="s">
-        <v>355</v>
-      </c>
       <c r="C54" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D54" s="18"/>
       <c r="E54" s="18"/>
@@ -11802,13 +11802,13 @@
     </row>
     <row r="55" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="B55" t="s">
         <v>356</v>
       </c>
-      <c r="B55" t="s">
-        <v>357</v>
-      </c>
       <c r="C55" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D55" s="18"/>
       <c r="E55" s="18"/>
@@ -11829,13 +11829,13 @@
     </row>
     <row r="56" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="B56" t="s">
         <v>358</v>
       </c>
-      <c r="B56" t="s">
-        <v>359</v>
-      </c>
       <c r="C56" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D56" s="18"/>
       <c r="E56" s="18"/>
@@ -11856,13 +11856,13 @@
     </row>
     <row r="57" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
+        <v>359</v>
+      </c>
+      <c r="B57" t="s">
         <v>360</v>
       </c>
-      <c r="B57" t="s">
-        <v>361</v>
-      </c>
       <c r="C57" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D57" s="18"/>
       <c r="E57" s="18"/>
@@ -11883,13 +11883,13 @@
     </row>
     <row r="58" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
+        <v>361</v>
+      </c>
+      <c r="B58" t="s">
         <v>362</v>
       </c>
-      <c r="B58" t="s">
-        <v>363</v>
-      </c>
       <c r="C58" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D58" s="18"/>
       <c r="E58" s="18"/>
@@ -11910,13 +11910,13 @@
     </row>
     <row r="59" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="B59" t="s">
         <v>364</v>
       </c>
-      <c r="B59" t="s">
-        <v>365</v>
-      </c>
       <c r="C59" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D59" s="18"/>
       <c r="E59" s="18"/>
@@ -11937,13 +11937,13 @@
     </row>
     <row r="60" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
+        <v>365</v>
+      </c>
+      <c r="B60" t="s">
         <v>366</v>
       </c>
-      <c r="B60" t="s">
-        <v>367</v>
-      </c>
       <c r="C60" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D60" s="18"/>
       <c r="E60" s="18"/>
@@ -11964,13 +11964,13 @@
     </row>
     <row r="61" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="B61" t="s">
         <v>368</v>
       </c>
-      <c r="B61" t="s">
-        <v>369</v>
-      </c>
       <c r="C61" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D61" s="18"/>
       <c r="E61" s="18"/>
@@ -11991,13 +11991,13 @@
     </row>
     <row r="62" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="18" t="s">
+        <v>369</v>
+      </c>
+      <c r="B62" t="s">
         <v>370</v>
       </c>
-      <c r="B62" t="s">
-        <v>371</v>
-      </c>
       <c r="C62" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D62" s="18"/>
       <c r="E62" s="18"/>
@@ -12018,13 +12018,13 @@
     </row>
     <row r="63" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
+        <v>371</v>
+      </c>
+      <c r="B63" t="s">
         <v>372</v>
       </c>
-      <c r="B63" t="s">
-        <v>373</v>
-      </c>
       <c r="C63" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D63" s="18"/>
       <c r="E63" s="18"/>
@@ -12045,13 +12045,13 @@
     </row>
     <row r="64" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="B64" t="s">
         <v>374</v>
       </c>
-      <c r="B64" t="s">
-        <v>375</v>
-      </c>
       <c r="C64" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D64" s="18"/>
       <c r="E64" s="18"/>
@@ -12072,13 +12072,13 @@
     </row>
     <row r="65" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
+        <v>375</v>
+      </c>
+      <c r="B65" t="s">
         <v>376</v>
       </c>
-      <c r="B65" t="s">
-        <v>377</v>
-      </c>
       <c r="C65" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D65" s="18"/>
       <c r="E65" s="18"/>
@@ -12099,13 +12099,13 @@
     </row>
     <row r="66" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="18" t="s">
+        <v>377</v>
+      </c>
+      <c r="B66" t="s">
         <v>378</v>
       </c>
-      <c r="B66" t="s">
-        <v>379</v>
-      </c>
       <c r="C66" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D66" s="18"/>
       <c r="E66" s="18"/>
@@ -12126,13 +12126,13 @@
     </row>
     <row r="67" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="18" t="s">
+        <v>379</v>
+      </c>
+      <c r="B67" t="s">
         <v>380</v>
       </c>
-      <c r="B67" t="s">
-        <v>381</v>
-      </c>
       <c r="C67" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D67" s="18"/>
       <c r="E67" s="18"/>
@@ -12153,13 +12153,13 @@
     </row>
     <row r="68" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
+        <v>381</v>
+      </c>
+      <c r="B68" t="s">
         <v>382</v>
       </c>
-      <c r="B68" t="s">
-        <v>383</v>
-      </c>
       <c r="C68" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D68" s="18"/>
       <c r="E68" s="18"/>
@@ -12180,13 +12180,13 @@
     </row>
     <row r="69" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="18" t="s">
+        <v>383</v>
+      </c>
+      <c r="B69" t="s">
         <v>384</v>
       </c>
-      <c r="B69" t="s">
-        <v>385</v>
-      </c>
       <c r="C69" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D69" s="18"/>
       <c r="E69" s="18"/>
@@ -12207,13 +12207,13 @@
     </row>
     <row r="70" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
+        <v>385</v>
+      </c>
+      <c r="B70" t="s">
         <v>386</v>
       </c>
-      <c r="B70" t="s">
-        <v>387</v>
-      </c>
       <c r="C70" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D70" s="18"/>
       <c r="E70" s="18"/>
@@ -12234,13 +12234,13 @@
     </row>
     <row r="71" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="B71" t="s">
         <v>388</v>
       </c>
-      <c r="B71" t="s">
-        <v>389</v>
-      </c>
       <c r="C71" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D71" s="18"/>
       <c r="E71" s="18"/>
@@ -12261,13 +12261,13 @@
     </row>
     <row r="72" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
+        <v>389</v>
+      </c>
+      <c r="B72" t="s">
         <v>390</v>
       </c>
-      <c r="B72" t="s">
-        <v>391</v>
-      </c>
       <c r="C72" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D72" s="18"/>
       <c r="E72" s="18"/>
@@ -12288,13 +12288,13 @@
     </row>
     <row r="73" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="B73" t="s">
         <v>392</v>
       </c>
-      <c r="B73" t="s">
-        <v>393</v>
-      </c>
       <c r="C73" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D73" s="18"/>
       <c r="E73" s="18"/>
@@ -12315,13 +12315,13 @@
     </row>
     <row r="74" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="18" t="s">
+        <v>393</v>
+      </c>
+      <c r="B74" t="s">
         <v>394</v>
       </c>
-      <c r="B74" t="s">
-        <v>395</v>
-      </c>
       <c r="C74" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D74" s="18"/>
       <c r="E74" s="18"/>
@@ -12342,13 +12342,13 @@
     </row>
     <row r="75" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="18" t="s">
+        <v>395</v>
+      </c>
+      <c r="B75" t="s">
         <v>396</v>
       </c>
-      <c r="B75" t="s">
-        <v>397</v>
-      </c>
       <c r="C75" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D75" s="18"/>
       <c r="E75" s="18"/>
@@ -12369,13 +12369,13 @@
     </row>
     <row r="76" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
+        <v>397</v>
+      </c>
+      <c r="B76" t="s">
         <v>398</v>
       </c>
-      <c r="B76" t="s">
-        <v>399</v>
-      </c>
       <c r="C76" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D76" s="18"/>
       <c r="E76" s="18"/>
@@ -12396,13 +12396,13 @@
     </row>
     <row r="77" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="B77" t="s">
         <v>400</v>
       </c>
-      <c r="B77" t="s">
-        <v>401</v>
-      </c>
       <c r="C77" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D77" s="18"/>
       <c r="E77" s="18"/>
@@ -12423,13 +12423,13 @@
     </row>
     <row r="78" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="18" t="s">
+        <v>401</v>
+      </c>
+      <c r="B78" t="s">
         <v>402</v>
       </c>
-      <c r="B78" t="s">
-        <v>403</v>
-      </c>
       <c r="C78" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D78" s="18"/>
       <c r="E78" s="18"/>
@@ -12450,13 +12450,13 @@
     </row>
     <row r="79" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="18" t="s">
+        <v>403</v>
+      </c>
+      <c r="B79" t="s">
         <v>404</v>
       </c>
-      <c r="B79" t="s">
-        <v>405</v>
-      </c>
       <c r="C79" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D79" s="18"/>
       <c r="E79" s="18"/>
@@ -12477,13 +12477,13 @@
     </row>
     <row r="80" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="18" t="s">
+        <v>405</v>
+      </c>
+      <c r="B80" t="s">
         <v>406</v>
       </c>
-      <c r="B80" t="s">
-        <v>407</v>
-      </c>
       <c r="C80" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D80" s="18"/>
       <c r="E80" s="18"/>
@@ -12504,13 +12504,13 @@
     </row>
     <row r="81" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="18" t="s">
+        <v>407</v>
+      </c>
+      <c r="B81" t="s">
         <v>408</v>
       </c>
-      <c r="B81" t="s">
-        <v>409</v>
-      </c>
       <c r="C81" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D81" s="18"/>
       <c r="E81" s="18"/>
@@ -12531,13 +12531,13 @@
     </row>
     <row r="82" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="B82" t="s">
         <v>410</v>
       </c>
-      <c r="B82" t="s">
-        <v>411</v>
-      </c>
       <c r="C82" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D82" s="18"/>
       <c r="E82" s="18"/>
@@ -12558,13 +12558,13 @@
     </row>
     <row r="83" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B83" t="s">
         <v>412</v>
       </c>
-      <c r="B83" t="s">
-        <v>413</v>
-      </c>
       <c r="C83" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D83" s="18"/>
       <c r="E83" s="18"/>
@@ -12585,13 +12585,13 @@
     </row>
     <row r="84" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="B84" t="s">
         <v>414</v>
       </c>
-      <c r="B84" t="s">
-        <v>415</v>
-      </c>
       <c r="C84" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D84" s="18"/>
       <c r="E84" s="18"/>
@@ -12612,13 +12612,13 @@
     </row>
     <row r="85" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="B85" t="s">
         <v>416</v>
       </c>
-      <c r="B85" t="s">
-        <v>417</v>
-      </c>
       <c r="C85" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D85" s="18"/>
       <c r="E85" s="18"/>
@@ -12639,13 +12639,13 @@
     </row>
     <row r="86" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="18" t="s">
+        <v>417</v>
+      </c>
+      <c r="B86" t="s">
         <v>418</v>
       </c>
-      <c r="B86" t="s">
-        <v>419</v>
-      </c>
       <c r="C86" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D86" s="18"/>
       <c r="E86" s="18"/>
@@ -12666,13 +12666,13 @@
     </row>
     <row r="87" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="18" t="s">
+        <v>419</v>
+      </c>
+      <c r="B87" t="s">
         <v>420</v>
       </c>
-      <c r="B87" t="s">
-        <v>421</v>
-      </c>
       <c r="C87" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D87" s="18"/>
       <c r="E87" s="18"/>
@@ -12693,13 +12693,13 @@
     </row>
     <row r="88" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="18" t="s">
+        <v>421</v>
+      </c>
+      <c r="B88" t="s">
         <v>422</v>
       </c>
-      <c r="B88" t="s">
-        <v>423</v>
-      </c>
       <c r="C88" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D88" s="18"/>
       <c r="E88" s="18"/>
@@ -12720,13 +12720,13 @@
     </row>
     <row r="89" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="B89" t="s">
         <v>424</v>
       </c>
-      <c r="B89" t="s">
-        <v>425</v>
-      </c>
       <c r="C89" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D89" s="18"/>
       <c r="E89" s="18"/>
@@ -12747,13 +12747,13 @@
     </row>
     <row r="90" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="18" t="s">
+        <v>425</v>
+      </c>
+      <c r="B90" t="s">
         <v>426</v>
       </c>
-      <c r="B90" t="s">
-        <v>427</v>
-      </c>
       <c r="C90" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D90" s="18"/>
       <c r="E90" s="18"/>
@@ -12774,13 +12774,13 @@
     </row>
     <row r="91" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="18" t="s">
+        <v>427</v>
+      </c>
+      <c r="B91" t="s">
         <v>428</v>
       </c>
-      <c r="B91" t="s">
-        <v>429</v>
-      </c>
       <c r="C91" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D91" s="18"/>
       <c r="E91" s="18"/>
@@ -12801,13 +12801,13 @@
     </row>
     <row r="92" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="18" t="s">
+        <v>429</v>
+      </c>
+      <c r="B92" t="s">
         <v>430</v>
       </c>
-      <c r="B92" t="s">
-        <v>431</v>
-      </c>
       <c r="C92" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D92" s="18"/>
       <c r="E92" s="18"/>
@@ -12828,13 +12828,13 @@
     </row>
     <row r="93" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="18" t="s">
+        <v>431</v>
+      </c>
+      <c r="B93" t="s">
         <v>432</v>
       </c>
-      <c r="B93" t="s">
-        <v>433</v>
-      </c>
       <c r="C93" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D93" s="18"/>
       <c r="E93" s="18"/>
@@ -12855,13 +12855,13 @@
     </row>
     <row r="94" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="18" t="s">
+        <v>433</v>
+      </c>
+      <c r="B94" t="s">
         <v>434</v>
       </c>
-      <c r="B94" t="s">
-        <v>435</v>
-      </c>
       <c r="C94" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D94" s="18"/>
       <c r="E94" s="18"/>
@@ -12882,13 +12882,13 @@
     </row>
     <row r="95" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="18" t="s">
+        <v>435</v>
+      </c>
+      <c r="B95" t="s">
         <v>436</v>
       </c>
-      <c r="B95" t="s">
-        <v>437</v>
-      </c>
       <c r="C95" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D95" s="18"/>
       <c r="E95" s="18"/>
@@ -12909,13 +12909,13 @@
     </row>
     <row r="96" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="18" t="s">
+        <v>437</v>
+      </c>
+      <c r="B96" t="s">
         <v>438</v>
       </c>
-      <c r="B96" t="s">
-        <v>439</v>
-      </c>
       <c r="C96" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D96" s="18"/>
       <c r="E96" s="18"/>
@@ -12936,13 +12936,13 @@
     </row>
     <row r="97" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="18" t="s">
+        <v>439</v>
+      </c>
+      <c r="B97" t="s">
         <v>440</v>
       </c>
-      <c r="B97" t="s">
-        <v>441</v>
-      </c>
       <c r="C97" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D97" s="18"/>
       <c r="E97" s="18"/>
@@ -12963,13 +12963,13 @@
     </row>
     <row r="98" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="18" t="s">
+        <v>441</v>
+      </c>
+      <c r="B98" t="s">
         <v>442</v>
       </c>
-      <c r="B98" t="s">
-        <v>443</v>
-      </c>
       <c r="C98" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D98" s="18"/>
       <c r="E98" s="18"/>
@@ -12990,13 +12990,13 @@
     </row>
     <row r="99" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="18" t="s">
+        <v>443</v>
+      </c>
+      <c r="B99" t="s">
         <v>444</v>
       </c>
-      <c r="B99" t="s">
-        <v>445</v>
-      </c>
       <c r="C99" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D99" s="18"/>
       <c r="E99" s="18"/>
@@ -13017,13 +13017,13 @@
     </row>
     <row r="100" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="18" t="s">
+        <v>445</v>
+      </c>
+      <c r="B100" t="s">
         <v>446</v>
       </c>
-      <c r="B100" t="s">
-        <v>447</v>
-      </c>
       <c r="C100" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D100" s="18"/>
       <c r="E100" s="18"/>
@@ -13044,13 +13044,13 @@
     </row>
     <row r="101" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="18" t="s">
+        <v>447</v>
+      </c>
+      <c r="B101" t="s">
         <v>448</v>
       </c>
-      <c r="B101" t="s">
-        <v>449</v>
-      </c>
       <c r="C101" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D101" s="18"/>
       <c r="E101" s="18"/>
@@ -13071,13 +13071,13 @@
     </row>
     <row r="102" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="18" t="s">
+        <v>449</v>
+      </c>
+      <c r="B102" t="s">
         <v>450</v>
       </c>
-      <c r="B102" t="s">
-        <v>451</v>
-      </c>
       <c r="C102" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D102" s="18"/>
       <c r="E102" s="18"/>
@@ -13098,13 +13098,13 @@
     </row>
     <row r="103" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="18" t="s">
+        <v>451</v>
+      </c>
+      <c r="B103" t="s">
         <v>452</v>
       </c>
-      <c r="B103" t="s">
-        <v>453</v>
-      </c>
       <c r="C103" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D103" s="18"/>
       <c r="E103" s="18"/>
@@ -13125,13 +13125,13 @@
     </row>
     <row r="104" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="18" t="s">
+        <v>453</v>
+      </c>
+      <c r="B104" t="s">
         <v>454</v>
       </c>
-      <c r="B104" t="s">
-        <v>455</v>
-      </c>
       <c r="C104" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D104" s="18"/>
       <c r="E104" s="18"/>
@@ -13152,13 +13152,13 @@
     </row>
     <row r="105" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="18" t="s">
+        <v>455</v>
+      </c>
+      <c r="B105" t="s">
         <v>456</v>
       </c>
-      <c r="B105" t="s">
-        <v>457</v>
-      </c>
       <c r="C105" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D105" s="18"/>
       <c r="E105" s="18"/>
@@ -13179,13 +13179,13 @@
     </row>
     <row r="106" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="18" t="s">
+        <v>457</v>
+      </c>
+      <c r="B106" t="s">
         <v>458</v>
       </c>
-      <c r="B106" t="s">
-        <v>459</v>
-      </c>
       <c r="C106" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D106" s="18"/>
       <c r="E106" s="18"/>
@@ -13206,13 +13206,13 @@
     </row>
     <row r="107" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="18" t="s">
+        <v>459</v>
+      </c>
+      <c r="B107" t="s">
         <v>460</v>
       </c>
-      <c r="B107" t="s">
-        <v>461</v>
-      </c>
       <c r="C107" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D107" s="18"/>
       <c r="E107" s="18"/>
@@ -13233,13 +13233,13 @@
     </row>
     <row r="108" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="18" t="s">
+        <v>461</v>
+      </c>
+      <c r="B108" t="s">
         <v>462</v>
       </c>
-      <c r="B108" t="s">
-        <v>463</v>
-      </c>
       <c r="C108" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D108" s="18"/>
       <c r="E108" s="18"/>
@@ -13260,13 +13260,13 @@
     </row>
     <row r="109" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="18" t="s">
+        <v>463</v>
+      </c>
+      <c r="B109" t="s">
         <v>464</v>
       </c>
-      <c r="B109" t="s">
-        <v>465</v>
-      </c>
       <c r="C109" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D109" s="18"/>
       <c r="E109" s="18"/>
@@ -13287,13 +13287,13 @@
     </row>
     <row r="110" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="18" t="s">
+        <v>465</v>
+      </c>
+      <c r="B110" t="s">
         <v>466</v>
       </c>
-      <c r="B110" t="s">
-        <v>467</v>
-      </c>
       <c r="C110" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D110" s="18"/>
       <c r="E110" s="18"/>
@@ -13314,13 +13314,13 @@
     </row>
     <row r="111" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="18" t="s">
+        <v>467</v>
+      </c>
+      <c r="B111" t="s">
         <v>468</v>
       </c>
-      <c r="B111" t="s">
-        <v>469</v>
-      </c>
       <c r="C111" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D111" s="18"/>
       <c r="E111" s="18"/>
@@ -13341,13 +13341,13 @@
     </row>
     <row r="112" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="18" t="s">
+        <v>469</v>
+      </c>
+      <c r="B112" t="s">
         <v>470</v>
       </c>
-      <c r="B112" t="s">
-        <v>471</v>
-      </c>
       <c r="C112" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D112" s="18"/>
       <c r="E112" s="18"/>
@@ -13368,13 +13368,13 @@
     </row>
     <row r="113" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="18" t="s">
+        <v>471</v>
+      </c>
+      <c r="B113" t="s">
         <v>472</v>
       </c>
-      <c r="B113" t="s">
-        <v>473</v>
-      </c>
       <c r="C113" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D113" s="18"/>
       <c r="E113" s="18"/>
@@ -13395,13 +13395,13 @@
     </row>
     <row r="114" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="18" t="s">
+        <v>473</v>
+      </c>
+      <c r="B114" t="s">
         <v>474</v>
       </c>
-      <c r="B114" t="s">
-        <v>475</v>
-      </c>
       <c r="C114" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D114" s="18"/>
       <c r="E114" s="18"/>
@@ -13422,13 +13422,13 @@
     </row>
     <row r="115" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="18" t="s">
+        <v>475</v>
+      </c>
+      <c r="B115" t="s">
         <v>476</v>
       </c>
-      <c r="B115" t="s">
-        <v>477</v>
-      </c>
       <c r="C115" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D115" s="18"/>
       <c r="E115" s="18"/>
@@ -13449,13 +13449,13 @@
     </row>
     <row r="116" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="18" t="s">
+        <v>477</v>
+      </c>
+      <c r="B116" t="s">
         <v>478</v>
       </c>
-      <c r="B116" t="s">
-        <v>479</v>
-      </c>
       <c r="C116" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D116" s="18"/>
       <c r="E116" s="18"/>
@@ -13476,13 +13476,13 @@
     </row>
     <row r="117" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="18" t="s">
+        <v>479</v>
+      </c>
+      <c r="B117" t="s">
         <v>480</v>
       </c>
-      <c r="B117" t="s">
-        <v>481</v>
-      </c>
       <c r="C117" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D117" s="18"/>
       <c r="E117" s="18"/>
@@ -13503,13 +13503,13 @@
     </row>
     <row r="118" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="18" t="s">
+        <v>481</v>
+      </c>
+      <c r="B118" t="s">
         <v>482</v>
       </c>
-      <c r="B118" t="s">
-        <v>483</v>
-      </c>
       <c r="C118" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D118" s="18"/>
       <c r="E118" s="18"/>
@@ -13530,13 +13530,13 @@
     </row>
     <row r="119" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="18" t="s">
+        <v>483</v>
+      </c>
+      <c r="B119" t="s">
         <v>484</v>
       </c>
-      <c r="B119" t="s">
-        <v>485</v>
-      </c>
       <c r="C119" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D119" s="18"/>
       <c r="E119" s="18"/>
@@ -13557,13 +13557,13 @@
     </row>
     <row r="120" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="18" t="s">
+        <v>485</v>
+      </c>
+      <c r="B120" t="s">
         <v>486</v>
       </c>
-      <c r="B120" t="s">
-        <v>487</v>
-      </c>
       <c r="C120" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D120" s="18"/>
       <c r="E120" s="18"/>
@@ -13584,13 +13584,13 @@
     </row>
     <row r="121" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="18" t="s">
+        <v>487</v>
+      </c>
+      <c r="B121" t="s">
         <v>488</v>
       </c>
-      <c r="B121" t="s">
-        <v>489</v>
-      </c>
       <c r="C121" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D121" s="18"/>
       <c r="E121" s="18"/>
@@ -13611,13 +13611,13 @@
     </row>
     <row r="122" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="18" t="s">
+        <v>489</v>
+      </c>
+      <c r="B122" t="s">
         <v>490</v>
       </c>
-      <c r="B122" t="s">
-        <v>491</v>
-      </c>
       <c r="C122" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D122" s="18"/>
       <c r="E122" s="18"/>
@@ -13638,13 +13638,13 @@
     </row>
     <row r="123" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="18" t="s">
+        <v>491</v>
+      </c>
+      <c r="B123" t="s">
         <v>492</v>
       </c>
-      <c r="B123" t="s">
-        <v>493</v>
-      </c>
       <c r="C123" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D123" s="18"/>
       <c r="E123" s="18"/>
@@ -13665,13 +13665,13 @@
     </row>
     <row r="124" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="B124" t="s">
         <v>494</v>
       </c>
-      <c r="B124" t="s">
-        <v>495</v>
-      </c>
       <c r="C124" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D124" s="18"/>
       <c r="E124" s="18"/>
@@ -14657,7 +14657,7 @@
   <dimension ref="A1:D103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D6" sqref="D6:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -14701,91 +14701,91 @@
         <v>17</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>266</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>249</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>267</v>
-      </c>
       <c r="D5" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>268</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>249</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>269</v>
-      </c>
       <c r="D6" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>252</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>271</v>
-      </c>
       <c r="D7" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>252</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>273</v>
-      </c>
       <c r="D8" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="C9" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="C9" s="18" t="s">
-        <v>276</v>
-      </c>
       <c r="D9" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="C10" s="18" t="s">
         <v>277</v>
       </c>
-      <c r="B10" s="18" t="s">
-        <v>275</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>278</v>
-      </c>
       <c r="D10" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -15450,29 +15450,29 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>219</v>
+      </c>
+      <c r="C4" s="46" t="s">
         <v>173</v>
       </c>
-      <c r="B4" s="42" t="s">
-        <v>220</v>
-      </c>
-      <c r="C4" s="46" t="s">
+      <c r="D4" s="17" t="s">
         <v>174</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>175</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
     </row>
     <row r="5" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="96" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="44">
         <v>0</v>
@@ -15481,10 +15481,10 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="96"/>
       <c r="B6" s="42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="44">
         <v>1</v>
@@ -15493,10 +15493,10 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="96"/>
       <c r="B7" s="42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="44">
         <v>0</v>
@@ -15505,10 +15505,10 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="96"/>
       <c r="B8" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" s="46" t="s">
         <v>171</v>
-      </c>
-      <c r="C8" s="46" t="s">
-        <v>172</v>
       </c>
       <c r="D8" s="44">
         <v>0</v>
@@ -15517,10 +15517,10 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="96"/>
       <c r="B9" s="42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" s="46" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="44">
         <v>1</v>
@@ -15529,10 +15529,10 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="96"/>
       <c r="B10" s="42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="44">
         <v>0</v>
@@ -15541,10 +15541,10 @@
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="96"/>
       <c r="B11" s="42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" s="46" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="44">
         <v>0</v>
@@ -15553,10 +15553,10 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="96"/>
       <c r="B12" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="44">
         <v>0</v>
@@ -15565,10 +15565,10 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="96"/>
       <c r="B13" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="44">
         <v>0</v>
@@ -15577,10 +15577,10 @@
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="96"/>
       <c r="B14" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="44">
         <v>0</v>
@@ -15589,10 +15589,10 @@
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="96"/>
       <c r="B15" s="42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="44">
         <v>100</v>
@@ -15600,13 +15600,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="96" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B16" s="42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="44">
         <v>0</v>
@@ -15615,10 +15615,10 @@
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="96"/>
       <c r="B17" s="42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="44">
         <v>1</v>
@@ -15627,10 +15627,10 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="96"/>
       <c r="B18" s="42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" s="44">
         <v>0</v>
@@ -15639,20 +15639,20 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="96"/>
       <c r="B19" s="43" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C19" s="47" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D19" s="45"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="96"/>
       <c r="B20" s="42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" s="44">
         <v>0</v>
@@ -15660,13 +15660,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="96" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" s="44">
         <v>1</v>
@@ -15675,10 +15675,10 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="96"/>
       <c r="B22" s="42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C22" s="46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" s="44">
         <v>1</v>
@@ -15687,10 +15687,10 @@
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="96"/>
       <c r="B23" s="42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C23" s="46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="44">
         <v>0</v>
@@ -15699,10 +15699,10 @@
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="96"/>
       <c r="B24" s="42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C24" s="46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24" s="44">
         <v>1</v>
@@ -15711,10 +15711,10 @@
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="96"/>
       <c r="B25" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25" s="46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="44">
         <v>20</v>
@@ -15723,10 +15723,10 @@
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="96"/>
       <c r="B26" s="42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C26" s="46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D26" s="44">
         <v>0</v>
@@ -15735,10 +15735,10 @@
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="96"/>
       <c r="B27" s="42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C27" s="46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D27" s="44">
         <v>1</v>
@@ -15747,10 +15747,10 @@
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="96"/>
       <c r="B28" s="42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C28" s="46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D28" s="44">
         <v>0</v>
@@ -15759,10 +15759,10 @@
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="96"/>
       <c r="B29" s="42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C29" s="46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D29" s="44">
         <v>2</v>
@@ -15771,10 +15771,10 @@
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="96"/>
       <c r="B30" s="42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C30" s="46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D30" s="44">
         <v>0</v>
@@ -15783,10 +15783,10 @@
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="96"/>
       <c r="B31" s="42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C31" s="46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D31" s="44">
         <v>1</v>
@@ -15794,13 +15794,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="96" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B32" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C32" s="46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D32" s="44">
         <v>25</v>
@@ -15809,10 +15809,10 @@
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="96"/>
       <c r="B33" s="42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C33" s="46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D33" s="44">
         <v>20</v>
@@ -15821,10 +15821,10 @@
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="96"/>
       <c r="B34" s="42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C34" s="46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D34" s="44">
         <v>1</v>
@@ -15833,10 +15833,10 @@
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="96"/>
       <c r="B35" s="42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C35" s="46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D35" s="44">
         <v>1</v>
@@ -15845,10 +15845,10 @@
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="96"/>
       <c r="B36" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C36" s="46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D36" s="44">
         <v>0.1</v>
@@ -15857,10 +15857,10 @@
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="96"/>
       <c r="B37" s="42" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C37" s="46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D37" s="44">
         <v>0</v>
@@ -15869,10 +15869,10 @@
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="96"/>
       <c r="B38" s="42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C38" s="46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D38" s="44">
         <v>1</v>
@@ -15881,10 +15881,10 @@
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="96"/>
       <c r="B39" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C39" s="46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D39" s="44">
         <v>0</v>
@@ -15892,13 +15892,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="96" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B40" s="42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C40" s="46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D40" s="44">
         <v>1</v>
@@ -15907,10 +15907,10 @@
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="96"/>
       <c r="B41" s="42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C41" s="46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D41" s="44">
         <v>1</v>
@@ -15919,10 +15919,10 @@
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="96"/>
       <c r="B42" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C42" s="46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D42" s="44">
         <v>1</v>
@@ -15931,10 +15931,10 @@
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="96"/>
       <c r="B43" s="42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C43" s="46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D43" s="44">
         <v>0</v>
@@ -15943,10 +15943,10 @@
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="96"/>
       <c r="B44" s="42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C44" s="46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D44" s="44">
         <v>80</v>
@@ -15955,10 +15955,10 @@
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="96"/>
       <c r="B45" s="42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C45" s="46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D45" s="44">
         <v>0.95</v>
@@ -15967,10 +15967,10 @@
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="96"/>
       <c r="B46" s="42" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C46" s="46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D46" s="44">
         <v>1.05</v>
@@ -15979,10 +15979,10 @@
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="96"/>
       <c r="B47" s="42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C47" s="46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D47" s="44">
         <v>1</v>
@@ -15990,13 +15990,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="96" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B48" s="42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C48" s="46" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D48" s="44">
         <v>100</v>
@@ -16005,10 +16005,10 @@
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="96"/>
       <c r="B49" s="42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C49" s="46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D49" s="44">
         <v>100</v>
@@ -16017,10 +16017,10 @@
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="96"/>
       <c r="B50" s="42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C50" s="46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D50" s="44">
         <v>100</v>
@@ -16028,13 +16028,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="96" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B51" s="42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C51" s="46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D51" s="44">
         <v>0</v>
@@ -16043,10 +16043,10 @@
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="96"/>
       <c r="B52" s="42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C52" s="46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D52" s="44">
         <v>0.9</v>
@@ -16055,10 +16055,10 @@
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="96"/>
       <c r="B53" s="42" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C53" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D53" s="44">
         <v>12</v>
@@ -16067,10 +16067,10 @@
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="96"/>
       <c r="B54" s="42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C54" s="46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D54" s="44">
         <v>0.95</v>
@@ -16079,10 +16079,10 @@
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="96"/>
       <c r="B55" s="42" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C55" s="46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D55" s="44">
         <v>0.1</v>
@@ -16091,10 +16091,10 @@
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="96"/>
       <c r="B56" s="42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C56" s="46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D56" s="44">
         <v>0</v>
@@ -16102,13 +16102,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="96" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B57" s="42" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C57" s="46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D57" s="44">
         <v>1</v>
@@ -16117,10 +16117,10 @@
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="96"/>
       <c r="B58" s="42" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C58" s="46" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D58" s="44">
         <v>0</v>
@@ -16176,7 +16176,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -16214,13 +16214,13 @@
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D4" s="17" t="b">
         <v>0</v>
@@ -16228,13 +16228,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="96" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D5" s="49">
         <v>50</v>
@@ -16243,10 +16243,10 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="96"/>
       <c r="B6" s="42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D6" s="44">
         <v>0</v>
@@ -16255,10 +16255,10 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="96"/>
       <c r="B7" s="42" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D7" s="49">
         <v>50</v>
@@ -16267,10 +16267,10 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="96"/>
       <c r="B8" s="42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C8" s="46" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D8" s="49">
         <v>2500</v>
@@ -16279,10 +16279,10 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="96"/>
       <c r="B9" s="42" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C9" s="46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D9" s="49">
         <v>5</v>
@@ -16291,10 +16291,10 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="96"/>
       <c r="B10" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D10" s="44">
         <v>0</v>
@@ -16302,13 +16302,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="96" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B11" s="42" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C11" s="46" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D11" s="44">
         <v>0.01</v>
@@ -16317,10 +16317,10 @@
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="96"/>
       <c r="B12" s="42" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D12" s="44">
         <v>5.0000000000000001E-3</v>
@@ -16329,10 +16329,10 @@
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="96"/>
       <c r="B13" s="42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D13" s="44">
         <v>10</v>
@@ -16341,10 +16341,10 @@
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="96"/>
       <c r="B14" s="42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D14" s="44">
         <v>0</v>
@@ -16396,8 +16396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6A76F2-659C-4442-872D-E00A53914A87}">
   <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -16413,7 +16413,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="98" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B1" s="98"/>
       <c r="C1" s="99"/>
@@ -16423,26 +16423,26 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="100" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B2" s="101"/>
       <c r="C2" s="102"/>
       <c r="D2" s="100" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E2" s="101"/>
       <c r="F2" s="102"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="103" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B3" s="104"/>
       <c r="C3" s="55">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D3" s="103" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E3" s="104"/>
       <c r="F3" s="56">
@@ -16452,14 +16452,14 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="103" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B4" s="104"/>
       <c r="C4" s="55">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D4" s="103" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E4" s="104"/>
       <c r="F4" s="56">
@@ -16469,14 +16469,14 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="105" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B5" s="106"/>
       <c r="C5" s="57">
         <v>15</v>
       </c>
       <c r="D5" s="105" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E5" s="106"/>
       <c r="F5" s="58">
@@ -16494,7 +16494,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="107" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B7" s="108"/>
       <c r="C7" s="108"/>
@@ -16504,22 +16504,22 @@
     </row>
     <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="62" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B8" s="63" t="s">
+        <v>226</v>
+      </c>
+      <c r="C8" s="64" t="s">
         <v>227</v>
       </c>
-      <c r="C8" s="64" t="s">
+      <c r="D8" s="63" t="s">
         <v>228</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="E8" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="F8" s="65" t="s">
         <v>229</v>
-      </c>
-      <c r="E8" s="63" t="s">
-        <v>226</v>
-      </c>
-      <c r="F8" s="65" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -18679,15 +18679,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
@@ -18698,7 +18689,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -18850,15 +18841,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -18874,7 +18866,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18890,4 +18882,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>